<commit_message>
Fix out incorrect geocoding
</commit_message>
<xml_diff>
--- a/ESW_data.xlsx
+++ b/ESW_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajulius/Documents/GitHub/eswglobal.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A2D2A3-B324-4B44-942C-0EA187B68B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A18483B-2C6F-654C-BA5D-92933F0AEE12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24680" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="248">
   <si>
     <t>State</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rochester, NY 14623</t>
   </si>
 </sst>
 </file>
@@ -805,18 +808,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1152,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1320,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>247</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
@@ -1465,7 +1457,7 @@
         <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="E11" t="s">
         <v>188</v>
@@ -1610,7 +1602,7 @@
         <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="E16" t="s">
         <v>115</v>
@@ -2016,7 +2008,7 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>215</v>
       </c>
       <c r="E30" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Add University of Illinois - Chicago
</commit_message>
<xml_diff>
--- a/ESW_data.xlsx
+++ b/ESW_data.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajulius/Documents/GitHub/eswglobal.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EEC74D-CC91-F24B-BE81-71FE724186F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E01A891-D796-DA4E-BA51-5C33C200BF88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24680" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="2880" windowWidth="24680" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
-  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="251">
   <si>
     <t>State</t>
   </si>
@@ -757,16 +754,25 @@
     <t>UCI</t>
   </si>
   <si>
-    <t>Area_Name</t>
-  </si>
-  <si>
     <t>Chapter_Locator</t>
   </si>
   <si>
+    <t>Rochester institute of technology (RIT)</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>1200 W Harrison St, Chicago, IL 60607</t>
+  </si>
+  <si>
+    <t>University of Illinois - Chicago</t>
+  </si>
+  <si>
+    <t>UIC</t>
+  </si>
+  <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>Rochester institute of technology (RIT)</t>
   </si>
 </sst>
 </file>
@@ -1141,22 +1147,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D7AB61-9C28-2C4D-86B1-F04E5D35E23F}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="84.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1170,13 +1176,13 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E1" t="s">
         <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G1" t="s">
         <v>57</v>
@@ -1205,10 +1211,10 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I2" t="s">
         <v>240</v>
@@ -1237,7 +1243,7 @@
         <v>123</v>
       </c>
       <c r="H3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I3" t="s">
         <v>240</v>
@@ -1312,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E6" t="s">
         <v>86</v>
@@ -1353,7 +1359,7 @@
         <v>139</v>
       </c>
       <c r="H7" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I7" t="s">
         <v>240</v>
@@ -1440,7 +1446,7 @@
         <v>144</v>
       </c>
       <c r="H10" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I10" t="s">
         <v>240</v>
@@ -1469,7 +1475,7 @@
         <v>189</v>
       </c>
       <c r="H11" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I11" t="s">
         <v>240</v>
@@ -1498,7 +1504,7 @@
         <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I12" t="s">
         <v>240</v>
@@ -1524,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H13" t="s">
         <v>167</v>
@@ -1611,10 +1617,10 @@
         <v>17</v>
       </c>
       <c r="G16" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H16" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="I16" t="s">
         <v>240</v>
@@ -1651,28 +1657,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>248</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>247</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>249</v>
       </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>250</v>
       </c>
       <c r="H18" t="s">
-        <v>158</v>
+        <v>250</v>
       </c>
       <c r="I18" t="s">
         <v>240</v>
@@ -1683,25 +1689,25 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
       <c r="F19" t="s">
         <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>246</v>
+        <v>132</v>
       </c>
       <c r="H19" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="I19" t="s">
         <v>240</v>
@@ -1709,28 +1715,28 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>241</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>250</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="I20" t="s">
         <v>240</v>
@@ -1738,28 +1744,28 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
       </c>
       <c r="G21" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="I21" t="s">
         <v>240</v>
@@ -1767,28 +1773,28 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
         <v>17</v>
       </c>
       <c r="G22" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="H22" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="I22" t="s">
         <v>240</v>
@@ -1796,28 +1802,28 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="H23" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="I23" t="s">
         <v>240</v>
@@ -1825,28 +1831,28 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="H24" t="s">
-        <v>171</v>
+        <v>250</v>
       </c>
       <c r="I24" t="s">
         <v>240</v>
@@ -1857,25 +1863,25 @@
         <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="H25" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="I25" t="s">
         <v>240</v>
@@ -1883,28 +1889,28 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
         <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>246</v>
+        <v>145</v>
       </c>
       <c r="H26" t="s">
-        <v>246</v>
+        <v>181</v>
       </c>
       <c r="I26" t="s">
         <v>240</v>
@@ -1915,25 +1921,25 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F27" t="s">
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="H27" t="s">
-        <v>183</v>
+        <v>250</v>
       </c>
       <c r="I27" t="s">
         <v>240</v>
@@ -1941,28 +1947,28 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="H28" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="I28" t="s">
         <v>240</v>
@@ -1970,28 +1976,28 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I29" t="s">
         <v>240</v>
@@ -1999,28 +2005,28 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
         <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H30" t="s">
-        <v>246</v>
+        <v>160</v>
       </c>
       <c r="I30" t="s">
         <v>240</v>
@@ -2028,28 +2034,28 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>246</v>
+        <v>125</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>250</v>
       </c>
       <c r="I31" t="s">
         <v>240</v>
@@ -2057,28 +2063,28 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C32" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>218</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="F32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G32" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I32" t="s">
         <v>240</v>
@@ -2086,28 +2092,28 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="F33" t="s">
         <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>192</v>
+        <v>250</v>
       </c>
       <c r="H33" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="I33" t="s">
         <v>240</v>
@@ -2115,28 +2121,28 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E34" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F34" t="s">
         <v>36</v>
       </c>
       <c r="G34" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="H34" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="I34" t="s">
         <v>240</v>
@@ -2147,25 +2153,25 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
         <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="H35" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="I35" t="s">
         <v>240</v>
@@ -2176,25 +2182,25 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="E36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
         <v>36</v>
       </c>
       <c r="G36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I36" t="s">
         <v>240</v>
@@ -2202,28 +2208,28 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="E37" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F37" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>246</v>
+        <v>151</v>
       </c>
       <c r="H37" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="I37" t="s">
         <v>240</v>
@@ -2231,28 +2237,28 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>235</v>
       </c>
       <c r="E38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
         <v>40</v>
       </c>
       <c r="G38" t="s">
-        <v>138</v>
+        <v>250</v>
       </c>
       <c r="H38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I38" t="s">
         <v>240</v>
@@ -2260,28 +2266,28 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
         <v>40</v>
       </c>
       <c r="G39" t="s">
-        <v>246</v>
+        <v>138</v>
       </c>
       <c r="H39" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="I39" t="s">
         <v>240</v>
@@ -2292,25 +2298,25 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="F40" t="s">
         <v>40</v>
       </c>
       <c r="G40" t="s">
-        <v>122</v>
+        <v>250</v>
       </c>
       <c r="H40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I40" t="s">
         <v>240</v>
@@ -2321,25 +2327,25 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
+        <v>70</v>
       </c>
       <c r="E41" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F41" t="s">
         <v>40</v>
       </c>
       <c r="G41" t="s">
-        <v>246</v>
+        <v>122</v>
       </c>
       <c r="H41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I41" t="s">
         <v>240</v>
@@ -2350,25 +2356,25 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>223</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="F42" t="s">
         <v>40</v>
       </c>
       <c r="G42" t="s">
-        <v>127</v>
+        <v>250</v>
       </c>
       <c r="H42" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I42" t="s">
         <v>240</v>
@@ -2379,25 +2385,25 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F43" t="s">
         <v>40</v>
       </c>
       <c r="G43" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H43" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="I43" t="s">
         <v>240</v>
@@ -2408,25 +2414,25 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F44" t="s">
         <v>40</v>
       </c>
       <c r="G44" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H44" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="I44" t="s">
         <v>240</v>
@@ -2437,25 +2443,25 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E45" t="s">
-        <v>243</v>
+        <v>101</v>
       </c>
       <c r="F45" t="s">
         <v>40</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I45" t="s">
         <v>240</v>
@@ -2466,25 +2472,25 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="F46" t="s">
         <v>40</v>
       </c>
       <c r="G46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I46" t="s">
         <v>240</v>
@@ -2495,32 +2501,60 @@
         <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F47" t="s">
         <v>40</v>
       </c>
       <c r="G47" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" t="s">
+        <v>179</v>
+      </c>
+      <c r="I47" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" t="s">
         <v>143</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>180</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I48" t="s">
         <v>240</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>